<commit_message>
refactor code task 30098
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
@@ -443,6 +443,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -464,26 +482,8 @@
     <xf numFmtId="168" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,7 +937,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -967,17 +967,17 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:11" ht="24" customHeight="1">
-      <c r="B3" s="44">
+      <c r="B3" s="37">
         <v>44015</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="49">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="41">
         <f>InvoiceTotal</f>
         <v>0</v>
       </c>
-      <c r="G3" s="49"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="3" t="s">
         <v>1</v>
       </c>
@@ -989,53 +989,53 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="46" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="46"/>
+      <c r="G6" s="50"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:11" ht="12.75" customHeight="1">
@@ -1139,8 +1139,8 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="42">
+      <c r="F19" s="46"/>
+      <c r="G19" s="48">
         <f>0</f>
         <v>0</v>
       </c>
@@ -1150,8 +1150,8 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="49"/>
     </row>
     <row r="22" spans="2:10" ht="15">
       <c r="B22" s="31" t="s">
@@ -1172,29 +1172,29 @@
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="2:10" ht="27" customHeight="1">
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
       <c r="J24" s="34"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F3:G4"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
30098 Project > Timesheet > Upgrade Export Invoice
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
@@ -33,6 +33,7 @@
     <definedName name="CompanySetup_YourName">INDEX(#REF!,MATCH("Your Name",#REF!,0))</definedName>
     <definedName name="CompanySetup_YourPhone">INDEX(#REF!,MATCH("Phone",#REF!,0))</definedName>
     <definedName name="CompanySetup_YourURL">INDEX(#REF!,MATCH("Website",#REF!,0))</definedName>
+    <definedName name="CurrencyInvoiceTotal" localSheetId="0">Invoice!$G$3</definedName>
     <definedName name="CurrencyTotal" localSheetId="0">Invoice!$F$19</definedName>
     <definedName name="DiaChiKhachHang" localSheetId="0">Invoice!$F$7</definedName>
     <definedName name="DiaChiKhachHang">Invoice!$F$7</definedName>
@@ -51,12 +52,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>INVOICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>NCCPLUS VIET NAM JOINT STOCK COMPANY</t>
@@ -114,15 +112,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="General;;"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00;;"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00;;\-"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00;;\-"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="8"/>
       <color theme="3"/>
@@ -239,6 +236,13 @@
     <font>
       <sz val="7"/>
       <color rgb="FF473530"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="4"/>
       <name val="Verdana"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -386,12 +390,6 @@
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -401,9 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -413,9 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -443,6 +435,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -452,18 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -476,14 +492,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,7 +511,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="#,##0.00;;"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -508,6 +521,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -517,6 +531,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
@@ -535,7 +550,7 @@
         <name val="Verdana"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="#,##0.00;;"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -937,7 +952,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="G19" sqref="G19:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -948,15 +963,15 @@
     <col min="4" max="4" width="23.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="27" style="3" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="4" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="3" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="3"/>
     <col min="11" max="11" width="20" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="27" customHeight="1"/>
-    <row r="2" spans="2:11" ht="43.5" customHeight="1">
+    <row r="2" spans="2:11" ht="43.5" customHeight="1" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -965,77 +980,78 @@
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="2:11" ht="24" customHeight="1">
-      <c r="B3" s="37">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:11" ht="24" customHeight="1" thickTop="1">
+      <c r="B3" s="45">
         <v>44015</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41">
-        <f>InvoiceTotal</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="2:11" ht="24" customHeight="1">
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="38" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="50"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="39" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40" t="s">
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="44" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:11" ht="12.75" customHeight="1">
@@ -1052,15 +1068,17 @@
       <c r="E11" s="8"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="2:11" ht="6" customHeight="1">
+    <row r="12" spans="2:11" ht="6" customHeight="1" thickBot="1">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="12"/>
       <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="2:11" ht="15" thickTop="1">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1068,133 +1086,143 @@
     </row>
     <row r="14" spans="2:11" ht="15">
       <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="18.75" customHeight="1">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="2:11" ht="18.75" customHeight="1">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="23">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="34">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="2:10" ht="18" customHeight="1">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="27">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="35">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="18" customHeight="1">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="27">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="35">
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:10" ht="18" customHeight="1">
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="48">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="18" customHeight="1">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="2:10" ht="18" customHeight="1" thickBot="1">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="49"/>
-    </row>
+      <c r="F20" s="51"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+    </row>
+    <row r="21" spans="2:10" ht="15" thickTop="1"/>
     <row r="22" spans="2:10" ht="15">
-      <c r="B22" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="B23" s="36"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" spans="2:10" ht="27" customHeight="1">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="J24" s="34"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="30"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="12">
-    <mergeCell ref="B24:G24"/>
+  <mergeCells count="16">
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F3:G4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
31037 31052 31032 31028 31081
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
@@ -335,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,12 +465,15 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -483,9 +486,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -497,6 +497,9 @@
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,7 +955,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:G20"/>
+      <selection activeCell="F7" sqref="F7:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -965,7 +968,8 @@
     <col min="6" max="6" width="19.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="22.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="3"/>
+    <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
     <col min="11" max="11" width="20" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -984,16 +988,16 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:11" ht="24" customHeight="1" thickTop="1">
-      <c r="B3" s="45">
+      <c r="B3" s="46">
         <v>44015</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
       <c r="F3" s="41"/>
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
-      <c r="I3" s="41"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="2:11" ht="24" customHeight="1">
       <c r="B4" s="6" t="s">
@@ -1005,54 +1009,59 @@
       <c r="F4" s="42"/>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
-      <c r="I4" s="42"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="43" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="44" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="2:11" ht="12.75" customHeight="1">
       <c r="B10" s="9"/>
@@ -1206,7 +1215,8 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="F7:I9"/>
     <mergeCell ref="B24:I24"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
@@ -1214,12 +1224,10 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>

</xml_diff>

<commit_message>
fix template excel invoice
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/Invoice.xlsx
@@ -16,21 +16,21 @@
     <sheet name="Detail" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ClientAddress" localSheetId="0">Invoice!$F$7</definedName>
-    <definedName name="ClientName" localSheetId="0">Invoice!$F$6</definedName>
+    <definedName name="ClientAddress" localSheetId="0">Invoice!$E$7</definedName>
+    <definedName name="ClientName" localSheetId="0">Invoice!$E$6</definedName>
     <definedName name="Currency" localSheetId="0">Invoice!$F$3</definedName>
     <definedName name="CurrencyTotal" localSheetId="0">Invoice!$F$19</definedName>
-    <definedName name="Discount" localSheetId="0">Invoice!$G$18</definedName>
-    <definedName name="DiscountLabel" localSheetId="0">Invoice!$F$18</definedName>
+    <definedName name="Discount" localSheetId="0">Invoice!$G$17</definedName>
+    <definedName name="DiscountLabel" localSheetId="0">Invoice!$F$17</definedName>
     <definedName name="InvoiceDate" localSheetId="0">Invoice!$B$3</definedName>
-    <definedName name="InvoiceNetTotal" localSheetId="0">Invoice!$G$17</definedName>
+    <definedName name="InvoiceNetTotal" localSheetId="0">Invoice!$G$16</definedName>
     <definedName name="InvoiceNumber" localSheetId="0">Invoice!$C$2</definedName>
     <definedName name="InvoiceNumberDisplay">Invoice!$E$2</definedName>
     <definedName name="InvoiceTotal" localSheetId="0">Invoice!$G$19</definedName>
     <definedName name="InvoiceTotalTop" localSheetId="0">Invoice!$G$3</definedName>
     <definedName name="PaymentDetails" localSheetId="0">Invoice!$B$23</definedName>
     <definedName name="PaymentDueBy" localSheetId="0">Invoice!$B$4</definedName>
-    <definedName name="TransferFee" localSheetId="0">Invoice!$G$16</definedName>
+    <definedName name="TransferFee" localSheetId="0">Invoice!$G$18</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -112,15 +112,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="General;;"/>
     <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="#,##0.00;;"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="8"/>
       <color theme="3"/>
@@ -171,13 +170,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="4"/>
       <name val="Verdana"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,17 +235,17 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="3"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="4"/>
       <name val="Verdana"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="3"/>
-      <name val="Sylfaen"/>
-      <family val="1"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -264,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -314,15 +306,6 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
         <color theme="1" tint="0.499984740745262"/>
       </top>
       <bottom/>
@@ -354,7 +337,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -373,10 +356,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -391,13 +374,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -406,17 +389,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -433,35 +407,26 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -481,16 +446,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -505,10 +470,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,44 +491,41 @@
     <xf numFmtId="3" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,7 +805,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="InvoiceDetails" displayName="InvoiceDetails" ref="B14:G15" insertRow="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="InvoiceDetails" displayName="InvoiceDetails" ref="B14:G15">
   <tableColumns count="6">
     <tableColumn id="1" name="NAME" dataDxfId="9"/>
     <tableColumn id="6" name="PROJECT" dataDxfId="8"/>
@@ -1090,116 +1061,115 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:I24"/>
+  <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="20" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="27" customHeight="1"/>
-    <row r="2" spans="2:9" ht="43.5" customHeight="1" thickBot="1">
+    <row r="1" spans="2:7" ht="27" customHeight="1"/>
+    <row r="2" spans="2:7" ht="43.5" customHeight="1" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="2:9" ht="24" customHeight="1" thickTop="1">
-      <c r="B3" s="64">
+    <row r="3" spans="2:7" ht="24" customHeight="1" thickTop="1">
+      <c r="B3" s="55">
         <v>44015</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="52"/>
-    </row>
-    <row r="4" spans="2:9" ht="24" customHeight="1">
+      <c r="C3" s="55"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="49"/>
+    </row>
+    <row r="4" spans="2:7" ht="24" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="53"/>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="57" t="s">
+      <c r="F4" s="52"/>
+      <c r="G4" s="50"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="56" t="s">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="56"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="58" t="s">
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="50" t="s">
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="50"/>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="59" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="59" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-    </row>
-    <row r="10" spans="2:9" ht="12.75" customHeight="1">
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+    </row>
+    <row r="10" spans="2:7" ht="12.75" customHeight="1">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="2:9" ht="6.75" customHeight="1">
+    <row r="11" spans="2:7" ht="6.75" customHeight="1">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="2:9" ht="6" customHeight="1" thickBot="1">
+    <row r="12" spans="2:7" ht="6" customHeight="1" thickBot="1">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1207,13 +1177,13 @@
       <c r="F12" s="12"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="2:9" ht="15" thickTop="1">
+    <row r="13" spans="2:7" ht="15" thickTop="1">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="2:9" ht="15">
+    <row r="14" spans="2:7" ht="15">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1226,120 +1196,118 @@
       <c r="E14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="34" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="18.75" customHeight="1">
+    <row r="15" spans="2:7" ht="18.75" customHeight="1">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-    </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1">
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="2:7" ht="18" customHeight="1">
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="34">
+        <v>8</v>
+      </c>
+      <c r="G16" s="45">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I16" s="31"/>
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="35">
+      <c r="F17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="45">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="18" customHeight="1">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="35">
-        <f>0</f>
+    <row r="18" spans="2:8" s="33" customFormat="1" ht="18" customHeight="1">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1">
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="62"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="61"/>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" thickBot="1">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="63"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="62"/>
     </row>
     <row r="21" spans="2:8" ht="15" thickTop="1"/>
     <row r="22" spans="2:8" ht="15">
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="2:8" ht="15">
-      <c r="B23" s="32"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="2:8" ht="27" customHeight="1">
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="30"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="27"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="F7:G9"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G9"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1360,55 +1328,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="4" style="37" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="48" customWidth="1"/>
-    <col min="4" max="4" width="20" style="37" customWidth="1"/>
-    <col min="5" max="5" width="52.42578125" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="37"/>
+    <col min="1" max="1" width="4" style="31" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="42" customWidth="1"/>
+    <col min="4" max="4" width="20" style="31" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="27">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-    </row>
-    <row r="3" spans="2:6" s="41" customFormat="1" ht="15">
-      <c r="B3" s="38" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+    </row>
+    <row r="3" spans="2:6" s="35" customFormat="1" ht="15">
+      <c r="B3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="39"/>
-    </row>
-    <row r="4" spans="2:6" s="41" customFormat="1" ht="18" customHeight="1">
-      <c r="B4" s="42"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="39"/>
+      <c r="F3" s="33"/>
+    </row>
+    <row r="4" spans="2:6" s="35" customFormat="1" ht="18" customHeight="1">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="2:6" ht="11.25" thickBot="1">
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:6" ht="11.25" thickTop="1">
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>